<commit_message>
Fixed insert request template
</commit_message>
<xml_diff>
--- a/AGD_共用維護Patrick.xlsx
+++ b/AGD_共用維護Patrick.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B114B730-60C0-4C47-BAEA-2996C9693771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087CD609-0ADD-4A4D-8E72-59D3FC0FD239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP_config" sheetId="9" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2788" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2788" uniqueCount="416">
   <si>
     <t>聯繫原因</t>
   </si>
@@ -1347,12 +1347,176 @@
     <t>原因ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>countryCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>authCallReason</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>aniCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skillCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reviewType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bussinessUnit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bussinessB03Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cBP83Note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>notificationType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ivrCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ctiStatus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kycCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>branchCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>marketingControl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sysConfig</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>country-code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>系統參數維護+A8AA2:B27</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>auth-call-reason</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ani-code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cit-status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill-code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>review-type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bussiness-unit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bussiness-b03-type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kyc-code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cbp83-note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ivr-code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>branch-code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>notification-type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>marketing-control</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sys-config</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1891,19 +2055,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.2"/>
   <cols>
     <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="19.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" s="8" t="s">
         <v>40</v>
       </c>
@@ -1920,7 +2084,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15" customHeight="1">
       <c r="A2" s="16" t="s">
         <v>223</v>
       </c>
@@ -1937,7 +2101,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15" customHeight="1">
       <c r="A3" s="16" t="s">
         <v>225</v>
       </c>
@@ -1945,16 +2109,16 @@
         <v>158</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>225</v>
+        <v>375</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>225</v>
+        <v>400</v>
       </c>
       <c r="F3" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15" customHeight="1">
       <c r="A4" s="16" t="s">
         <v>226</v>
       </c>
@@ -1962,16 +2126,16 @@
         <v>159</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>226</v>
+        <v>376</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>226</v>
+        <v>402</v>
       </c>
       <c r="F4" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15" customHeight="1">
       <c r="A5" s="16" t="s">
         <v>227</v>
       </c>
@@ -1979,16 +2143,16 @@
         <v>161</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>227</v>
+        <v>385</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>227</v>
+        <v>404</v>
       </c>
       <c r="F5" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="15" customHeight="1">
       <c r="A6" s="16" t="s">
         <v>228</v>
       </c>
@@ -1996,16 +2160,16 @@
         <v>162</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>228</v>
+        <v>377</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>228</v>
+        <v>403</v>
       </c>
       <c r="F6" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15" customHeight="1">
       <c r="A7" s="16" t="s">
         <v>229</v>
       </c>
@@ -2013,16 +2177,16 @@
         <v>163</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>229</v>
+        <v>378</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>229</v>
+        <v>405</v>
       </c>
       <c r="F7" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15" customHeight="1">
       <c r="A8" s="16" t="s">
         <v>230</v>
       </c>
@@ -2030,16 +2194,16 @@
         <v>165</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>230</v>
+        <v>384</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>230</v>
+        <v>411</v>
       </c>
       <c r="F8" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15" customHeight="1">
       <c r="A9" s="16" t="s">
         <v>231</v>
       </c>
@@ -2047,16 +2211,16 @@
         <v>168</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>231</v>
+        <v>379</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>231</v>
+        <v>406</v>
       </c>
       <c r="F9" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15" customHeight="1">
       <c r="A10" s="16" t="s">
         <v>232</v>
       </c>
@@ -2064,16 +2228,16 @@
         <v>169</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>232</v>
+        <v>380</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>232</v>
+        <v>407</v>
       </c>
       <c r="F10" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>233</v>
       </c>
@@ -2081,16 +2245,16 @@
         <v>170</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>233</v>
+        <v>381</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>233</v>
+        <v>408</v>
       </c>
       <c r="F11" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="15" customHeight="1">
       <c r="A12" s="16" t="s">
         <v>234</v>
       </c>
@@ -2098,16 +2262,16 @@
         <v>171</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>234</v>
+        <v>386</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>234</v>
+        <v>409</v>
       </c>
       <c r="F12" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="15" customHeight="1">
       <c r="A13" s="16" t="s">
         <v>235</v>
       </c>
@@ -2115,16 +2279,16 @@
         <v>172</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>235</v>
+        <v>382</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>235</v>
+        <v>410</v>
       </c>
       <c r="F13" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="15" customHeight="1">
       <c r="A14" s="16" t="s">
         <v>236</v>
       </c>
@@ -2132,16 +2296,16 @@
         <v>173</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>236</v>
+        <v>387</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>236</v>
+        <v>412</v>
       </c>
       <c r="F14" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="15" customHeight="1">
       <c r="A15" s="16" t="s">
         <v>237</v>
       </c>
@@ -2149,16 +2313,16 @@
         <v>176</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>237</v>
+        <v>383</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>237</v>
+        <v>413</v>
       </c>
       <c r="F15" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="15" customHeight="1">
       <c r="A16" s="16" t="s">
         <v>238</v>
       </c>
@@ -2166,16 +2330,16 @@
         <v>182</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>238</v>
+        <v>388</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>238</v>
+        <v>388</v>
       </c>
       <c r="F16" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="15" customHeight="1">
       <c r="A17" s="16" t="s">
         <v>239</v>
       </c>
@@ -2183,16 +2347,16 @@
         <v>184</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>239</v>
+        <v>389</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>239</v>
+        <v>389</v>
       </c>
       <c r="F17" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="15" customHeight="1">
       <c r="A18" s="16" t="s">
         <v>240</v>
       </c>
@@ -2200,16 +2364,16 @@
         <v>186</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>240</v>
+        <v>390</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>240</v>
+        <v>390</v>
       </c>
       <c r="F18" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="15" customHeight="1">
       <c r="A19" s="16" t="s">
         <v>241</v>
       </c>
@@ -2217,16 +2381,16 @@
         <v>213</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>241</v>
+        <v>391</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>241</v>
+        <v>391</v>
       </c>
       <c r="F19" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="15" customHeight="1">
       <c r="A20" s="16" t="s">
         <v>242</v>
       </c>
@@ -2234,16 +2398,16 @@
         <v>193</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>242</v>
+        <v>392</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>242</v>
+        <v>414</v>
       </c>
       <c r="F20" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="15" customHeight="1">
       <c r="A21" s="16" t="s">
         <v>289</v>
       </c>
@@ -2251,16 +2415,16 @@
         <v>194</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>289</v>
+        <v>393</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>289</v>
+        <v>393</v>
       </c>
       <c r="F21" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="15" customHeight="1">
       <c r="A22" s="16" t="s">
         <v>290</v>
       </c>
@@ -2268,16 +2432,16 @@
         <v>195</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>290</v>
+        <v>395</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>290</v>
+        <v>395</v>
       </c>
       <c r="F22" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="15" customHeight="1">
       <c r="A23" s="16" t="s">
         <v>291</v>
       </c>
@@ -2285,16 +2449,16 @@
         <v>196</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>291</v>
+        <v>394</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>291</v>
+        <v>394</v>
       </c>
       <c r="F23" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="15" customHeight="1">
       <c r="A24" s="16" t="s">
         <v>292</v>
       </c>
@@ -2302,16 +2466,16 @@
         <v>197</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>292</v>
+        <v>396</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>292</v>
+        <v>396</v>
       </c>
       <c r="F24" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="15" customHeight="1">
       <c r="A25" s="16" t="s">
         <v>293</v>
       </c>
@@ -2319,16 +2483,16 @@
         <v>198</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>293</v>
+        <v>397</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>293</v>
+        <v>397</v>
       </c>
       <c r="F25" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="15" customHeight="1">
       <c r="A26" s="16" t="s">
         <v>294</v>
       </c>
@@ -2336,27 +2500,27 @@
         <v>199</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>294</v>
+        <v>398</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>294</v>
+        <v>398</v>
       </c>
       <c r="F26" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="15" customHeight="1">
       <c r="A27" s="16" t="s">
         <v>32</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>1</v>
+        <v>401</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>32</v>
+        <v>399</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>32</v>
+        <v>415</v>
       </c>
       <c r="F27" t="s">
         <v>137</v>
@@ -2373,13 +2537,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y339"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.2"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="2" customWidth="1"/>
     <col min="2" max="2" width="31" style="2" bestFit="1" customWidth="1"/>
@@ -2405,7 +2569,7 @@
     <col min="25" max="25" width="12.21875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25">
       <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
@@ -2482,7 +2646,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25">
       <c r="A2" s="7" t="s">
         <v>15</v>
       </c>
@@ -2522,7 +2686,7 @@
       </c>
       <c r="Y2"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25">
       <c r="A3" s="7" t="s">
         <v>15</v>
       </c>
@@ -2568,7 +2732,7 @@
       </c>
       <c r="Y3"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -2626,7 +2790,7 @@
       </c>
       <c r="Y4"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25">
       <c r="A5" s="7" t="s">
         <v>15</v>
       </c>
@@ -2679,7 +2843,7 @@
       </c>
       <c r="Y5"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25">
       <c r="A6" s="7" t="s">
         <v>15</v>
       </c>
@@ -2720,7 +2884,7 @@
       <c r="U6"/>
       <c r="Y6"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25">
       <c r="A7" s="7" t="s">
         <v>15</v>
       </c>
@@ -2761,7 +2925,7 @@
       <c r="U7"/>
       <c r="Y7"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25">
       <c r="A8" s="7" t="s">
         <v>15</v>
       </c>
@@ -2804,7 +2968,7 @@
       </c>
       <c r="Y8"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25">
       <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
@@ -2843,7 +3007,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25">
       <c r="A10" s="7" t="s">
         <v>15</v>
       </c>
@@ -2877,7 +3041,7 @@
       <c r="U10"/>
       <c r="Y10"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25">
       <c r="A11" s="7" t="s">
         <v>15</v>
       </c>
@@ -2911,7 +3075,7 @@
       <c r="U11"/>
       <c r="Y11"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25">
       <c r="A12" s="7" t="s">
         <v>15</v>
       </c>
@@ -2945,7 +3109,7 @@
       <c r="U12"/>
       <c r="Y12"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25">
       <c r="A13" s="7" t="s">
         <v>15</v>
       </c>
@@ -2982,7 +3146,7 @@
       <c r="U13"/>
       <c r="Y13"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25">
       <c r="A14" s="7" t="s">
         <v>15</v>
       </c>
@@ -3019,7 +3183,7 @@
       <c r="U14"/>
       <c r="Y14"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25">
       <c r="A15" s="7" t="s">
         <v>15</v>
       </c>
@@ -3056,7 +3220,7 @@
       <c r="U15"/>
       <c r="Y15"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25">
       <c r="A16" s="7" t="s">
         <v>15</v>
       </c>
@@ -3096,7 +3260,7 @@
       </c>
       <c r="Y16"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25">
       <c r="A17" s="7" t="s">
         <v>15</v>
       </c>
@@ -3142,7 +3306,7 @@
       </c>
       <c r="Y17"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25">
       <c r="A18" s="7" t="s">
         <v>15</v>
       </c>
@@ -3200,7 +3364,7 @@
       </c>
       <c r="Y18"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25">
       <c r="A19" s="7" t="s">
         <v>15</v>
       </c>
@@ -3253,7 +3417,7 @@
       </c>
       <c r="Y19"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25">
       <c r="A20" s="7" t="s">
         <v>15</v>
       </c>
@@ -3294,7 +3458,7 @@
       <c r="U20"/>
       <c r="Y20"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25">
       <c r="A21" s="7" t="s">
         <v>15</v>
       </c>
@@ -3335,7 +3499,7 @@
       <c r="U21"/>
       <c r="Y21"/>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25">
       <c r="A22" s="7" t="s">
         <v>15</v>
       </c>
@@ -3372,7 +3536,7 @@
       <c r="U22"/>
       <c r="Y22"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25">
       <c r="A23" s="7" t="s">
         <v>15</v>
       </c>
@@ -3411,7 +3575,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:25">
       <c r="A24" s="7" t="s">
         <v>15</v>
       </c>
@@ -3445,7 +3609,7 @@
       <c r="U24"/>
       <c r="Y24"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:25">
       <c r="A25" s="7" t="s">
         <v>15</v>
       </c>
@@ -3479,7 +3643,7 @@
       <c r="U25"/>
       <c r="Y25"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:25">
       <c r="A26" s="7" t="s">
         <v>15</v>
       </c>
@@ -3513,7 +3677,7 @@
       <c r="U26"/>
       <c r="Y26"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:25">
       <c r="A27" s="7" t="s">
         <v>15</v>
       </c>
@@ -3550,7 +3714,7 @@
       <c r="U27"/>
       <c r="Y27"/>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:25">
       <c r="A28" s="7" t="s">
         <v>15</v>
       </c>
@@ -3587,7 +3751,7 @@
       <c r="U28"/>
       <c r="Y28"/>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:25">
       <c r="A29" s="7" t="s">
         <v>15</v>
       </c>
@@ -3624,7 +3788,7 @@
       <c r="U29"/>
       <c r="Y29"/>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:25">
       <c r="A30" s="7" t="s">
         <v>15</v>
       </c>
@@ -3664,7 +3828,7 @@
       </c>
       <c r="Y30"/>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:25">
       <c r="A31" s="7" t="s">
         <v>15</v>
       </c>
@@ -3710,7 +3874,7 @@
       </c>
       <c r="Y31"/>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:25">
       <c r="A32" s="7" t="s">
         <v>15</v>
       </c>
@@ -3768,7 +3932,7 @@
       </c>
       <c r="Y32"/>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:25">
       <c r="A33" s="7" t="s">
         <v>15</v>
       </c>
@@ -3821,7 +3985,7 @@
       </c>
       <c r="Y33"/>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:25">
       <c r="A34" s="7" t="s">
         <v>15</v>
       </c>
@@ -3862,7 +4026,7 @@
       <c r="U34"/>
       <c r="Y34"/>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:25">
       <c r="A35" s="7" t="s">
         <v>15</v>
       </c>
@@ -3903,7 +4067,7 @@
       <c r="U35"/>
       <c r="Y35"/>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:25">
       <c r="A36" s="7" t="s">
         <v>15</v>
       </c>
@@ -3940,7 +4104,7 @@
       <c r="U36"/>
       <c r="Y36"/>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:25">
       <c r="A37" s="7" t="s">
         <v>15</v>
       </c>
@@ -3979,7 +4143,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:25">
       <c r="A38" s="7" t="s">
         <v>15</v>
       </c>
@@ -4013,7 +4177,7 @@
       <c r="U38"/>
       <c r="Y38"/>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:25">
       <c r="A39" s="7" t="s">
         <v>15</v>
       </c>
@@ -4047,7 +4211,7 @@
       <c r="U39"/>
       <c r="Y39"/>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:25">
       <c r="A40" s="7" t="s">
         <v>15</v>
       </c>
@@ -4081,7 +4245,7 @@
       <c r="U40"/>
       <c r="Y40"/>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:25">
       <c r="A41" s="7" t="s">
         <v>15</v>
       </c>
@@ -4118,7 +4282,7 @@
       <c r="U41"/>
       <c r="Y41"/>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:25">
       <c r="A42" s="7" t="s">
         <v>15</v>
       </c>
@@ -4155,7 +4319,7 @@
       <c r="U42"/>
       <c r="Y42"/>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:25">
       <c r="A43" s="7" t="s">
         <v>15</v>
       </c>
@@ -4192,7 +4356,7 @@
       <c r="U43"/>
       <c r="Y43"/>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:25">
       <c r="A44" s="7" t="s">
         <v>15</v>
       </c>
@@ -4224,7 +4388,7 @@
       <c r="U44"/>
       <c r="Y44"/>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:25">
       <c r="A45" s="7" t="s">
         <v>15</v>
       </c>
@@ -4256,7 +4420,7 @@
       <c r="N45"/>
       <c r="Y45"/>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:25">
       <c r="A46" s="7" t="s">
         <v>15</v>
       </c>
@@ -4312,7 +4476,7 @@
       </c>
       <c r="Y46"/>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:25">
       <c r="A47" s="7" t="s">
         <v>15</v>
       </c>
@@ -4365,7 +4529,7 @@
       </c>
       <c r="Y47"/>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:25">
       <c r="A48" s="7" t="s">
         <v>15</v>
       </c>
@@ -4418,7 +4582,7 @@
       </c>
       <c r="Y48"/>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:25">
       <c r="A49" s="7" t="s">
         <v>15</v>
       </c>
@@ -4469,7 +4633,7 @@
       </c>
       <c r="Y49"/>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:25">
       <c r="A50" s="7" t="s">
         <v>15</v>
       </c>
@@ -4510,7 +4674,7 @@
       <c r="U50"/>
       <c r="Y50"/>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:25">
       <c r="A51" s="7" t="s">
         <v>15</v>
       </c>
@@ -4551,7 +4715,7 @@
       <c r="U51"/>
       <c r="Y51"/>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:25">
       <c r="A52" s="7" t="s">
         <v>15</v>
       </c>
@@ -4590,7 +4754,7 @@
       <c r="U52"/>
       <c r="Y52"/>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:25">
       <c r="A53" s="7" t="s">
         <v>15</v>
       </c>
@@ -4634,7 +4798,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:25">
       <c r="A54" s="7" t="s">
         <v>15</v>
       </c>
@@ -4671,7 +4835,7 @@
       <c r="U54"/>
       <c r="Y54"/>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:25">
       <c r="A55" s="7" t="s">
         <v>15</v>
       </c>
@@ -4708,7 +4872,7 @@
       <c r="U55"/>
       <c r="Y55"/>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:25">
       <c r="A56" s="7" t="s">
         <v>15</v>
       </c>
@@ -4748,7 +4912,7 @@
       </c>
       <c r="Y56"/>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:25">
       <c r="A57" s="7" t="s">
         <v>15</v>
       </c>
@@ -4794,7 +4958,7 @@
       </c>
       <c r="Y57"/>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:25">
       <c r="A58" s="7" t="s">
         <v>15</v>
       </c>
@@ -4852,7 +5016,7 @@
       </c>
       <c r="Y58"/>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:25">
       <c r="A59" s="7" t="s">
         <v>15</v>
       </c>
@@ -4905,7 +5069,7 @@
       </c>
       <c r="Y59"/>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:25">
       <c r="A60" s="7" t="s">
         <v>15</v>
       </c>
@@ -4946,7 +5110,7 @@
       <c r="U60"/>
       <c r="Y60"/>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:25">
       <c r="A61" s="7" t="s">
         <v>15</v>
       </c>
@@ -4987,7 +5151,7 @@
       <c r="U61"/>
       <c r="Y61"/>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:25">
       <c r="A62" s="7" t="s">
         <v>15</v>
       </c>
@@ -5024,7 +5188,7 @@
       <c r="U62"/>
       <c r="Y62"/>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:25">
       <c r="A63" s="7" t="s">
         <v>15</v>
       </c>
@@ -5063,7 +5227,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:25">
       <c r="A64" s="7" t="s">
         <v>15</v>
       </c>
@@ -5097,7 +5261,7 @@
       <c r="U64"/>
       <c r="Y64"/>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:25">
       <c r="A65" s="7" t="s">
         <v>15</v>
       </c>
@@ -5131,7 +5295,7 @@
       <c r="U65"/>
       <c r="Y65"/>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:25">
       <c r="A66" s="7" t="s">
         <v>15</v>
       </c>
@@ -5165,7 +5329,7 @@
       <c r="U66"/>
       <c r="Y66"/>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:25">
       <c r="A67" s="7" t="s">
         <v>15</v>
       </c>
@@ -5202,7 +5366,7 @@
       <c r="U67"/>
       <c r="Y67"/>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:25">
       <c r="A68" s="7" t="s">
         <v>15</v>
       </c>
@@ -5239,7 +5403,7 @@
       <c r="U68"/>
       <c r="Y68"/>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:25">
       <c r="A69" s="7" t="s">
         <v>15</v>
       </c>
@@ -5276,7 +5440,7 @@
       <c r="U69"/>
       <c r="Y69"/>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:25">
       <c r="A70" s="7" t="s">
         <v>15</v>
       </c>
@@ -5316,7 +5480,7 @@
       </c>
       <c r="Y70"/>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:25">
       <c r="A71" s="7" t="s">
         <v>15</v>
       </c>
@@ -5362,7 +5526,7 @@
       </c>
       <c r="Y71"/>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:25">
       <c r="A72" s="7" t="s">
         <v>15</v>
       </c>
@@ -5420,7 +5584,7 @@
       </c>
       <c r="Y72"/>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:25">
       <c r="A73" s="7" t="s">
         <v>15</v>
       </c>
@@ -5473,7 +5637,7 @@
       </c>
       <c r="Y73"/>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:25">
       <c r="A74" s="7" t="s">
         <v>15</v>
       </c>
@@ -5514,7 +5678,7 @@
       <c r="U74"/>
       <c r="Y74"/>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:25">
       <c r="A75" s="7" t="s">
         <v>15</v>
       </c>
@@ -5555,7 +5719,7 @@
       <c r="U75"/>
       <c r="Y75"/>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:25">
       <c r="A76" s="7" t="s">
         <v>15</v>
       </c>
@@ -5592,7 +5756,7 @@
       <c r="U76"/>
       <c r="Y76"/>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:25">
       <c r="A77" s="7" t="s">
         <v>15</v>
       </c>
@@ -5631,7 +5795,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:25">
       <c r="A78" s="7" t="s">
         <v>15</v>
       </c>
@@ -5665,7 +5829,7 @@
       <c r="U78"/>
       <c r="Y78"/>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:25">
       <c r="A79" s="7" t="s">
         <v>15</v>
       </c>
@@ -5699,7 +5863,7 @@
       <c r="U79"/>
       <c r="Y79"/>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:25">
       <c r="A80" s="7" t="s">
         <v>15</v>
       </c>
@@ -5733,7 +5897,7 @@
       <c r="U80"/>
       <c r="Y80"/>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:25">
       <c r="A81" s="7" t="s">
         <v>15</v>
       </c>
@@ -5770,7 +5934,7 @@
       <c r="U81"/>
       <c r="Y81"/>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:25">
       <c r="A82" s="7" t="s">
         <v>15</v>
       </c>
@@ -5807,7 +5971,7 @@
       <c r="U82"/>
       <c r="Y82"/>
     </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:25">
       <c r="A83" s="7" t="s">
         <v>15</v>
       </c>
@@ -5844,7 +6008,7 @@
       <c r="U83"/>
       <c r="Y83"/>
     </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:25">
       <c r="A84" s="7" t="s">
         <v>15</v>
       </c>
@@ -5884,7 +6048,7 @@
       </c>
       <c r="Y84"/>
     </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:25">
       <c r="A85" s="7" t="s">
         <v>15</v>
       </c>
@@ -5930,7 +6094,7 @@
       </c>
       <c r="Y85"/>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:25">
       <c r="A86" s="7" t="s">
         <v>15</v>
       </c>
@@ -5988,7 +6152,7 @@
       </c>
       <c r="Y86"/>
     </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:25">
       <c r="A87" s="7" t="s">
         <v>15</v>
       </c>
@@ -6041,7 +6205,7 @@
       </c>
       <c r="Y87"/>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:25">
       <c r="A88" s="7" t="s">
         <v>15</v>
       </c>
@@ -6091,7 +6255,7 @@
       </c>
       <c r="Y88"/>
     </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:25">
       <c r="A89" s="7" t="s">
         <v>15</v>
       </c>
@@ -6126,7 +6290,7 @@
       <c r="U89"/>
       <c r="Y89"/>
     </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:25">
       <c r="A90" s="7" t="s">
         <v>15</v>
       </c>
@@ -6157,7 +6321,7 @@
       <c r="U90"/>
       <c r="Y90"/>
     </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:25">
       <c r="A91" s="7" t="s">
         <v>15</v>
       </c>
@@ -6190,7 +6354,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:25">
       <c r="A92" s="7" t="s">
         <v>15</v>
       </c>
@@ -6224,7 +6388,7 @@
       <c r="U92"/>
       <c r="Y92"/>
     </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:25">
       <c r="A93" s="7" t="s">
         <v>15</v>
       </c>
@@ -6258,7 +6422,7 @@
       <c r="U93"/>
       <c r="Y93"/>
     </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:25">
       <c r="A94" s="7" t="s">
         <v>15</v>
       </c>
@@ -6292,7 +6456,7 @@
       <c r="U94"/>
       <c r="Y94"/>
     </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:25">
       <c r="A95" s="7" t="s">
         <v>15</v>
       </c>
@@ -6329,7 +6493,7 @@
       <c r="U95"/>
       <c r="Y95"/>
     </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:25">
       <c r="A96" s="7" t="s">
         <v>15</v>
       </c>
@@ -6366,7 +6530,7 @@
       <c r="U96"/>
       <c r="Y96"/>
     </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:25">
       <c r="A97" s="7" t="s">
         <v>15</v>
       </c>
@@ -6403,7 +6567,7 @@
       <c r="U97"/>
       <c r="Y97"/>
     </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:25">
       <c r="A98" s="7" t="s">
         <v>15</v>
       </c>
@@ -6443,7 +6607,7 @@
       </c>
       <c r="Y98"/>
     </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:25">
       <c r="A99" s="7" t="s">
         <v>15</v>
       </c>
@@ -6489,7 +6653,7 @@
       </c>
       <c r="Y99"/>
     </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:25">
       <c r="A100" s="7" t="s">
         <v>15</v>
       </c>
@@ -6547,7 +6711,7 @@
       </c>
       <c r="Y100"/>
     </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:25">
       <c r="A101" s="7" t="s">
         <v>15</v>
       </c>
@@ -6600,7 +6764,7 @@
       </c>
       <c r="Y101"/>
     </row>
-    <row r="102" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:25">
       <c r="A102" s="7" t="s">
         <v>15</v>
       </c>
@@ -6635,7 +6799,7 @@
       <c r="U102"/>
       <c r="Y102"/>
     </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:25">
       <c r="A103" s="7" t="s">
         <v>15</v>
       </c>
@@ -6670,7 +6834,7 @@
       <c r="U103"/>
       <c r="Y103"/>
     </row>
-    <row r="104" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:25">
       <c r="A104" s="7" t="s">
         <v>15</v>
       </c>
@@ -6701,7 +6865,7 @@
       <c r="U104"/>
       <c r="Y104"/>
     </row>
-    <row r="105" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:25">
       <c r="A105" s="7" t="s">
         <v>15</v>
       </c>
@@ -6743,7 +6907,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="106" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:25">
       <c r="A106" s="7" t="s">
         <v>15</v>
       </c>
@@ -6777,7 +6941,7 @@
       <c r="U106"/>
       <c r="Y106"/>
     </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:25">
       <c r="A107" s="7" t="s">
         <v>15</v>
       </c>
@@ -6811,7 +6975,7 @@
       <c r="U107"/>
       <c r="Y107"/>
     </row>
-    <row r="108" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:25">
       <c r="A108" s="7" t="s">
         <v>15</v>
       </c>
@@ -6845,7 +7009,7 @@
       <c r="U108"/>
       <c r="Y108"/>
     </row>
-    <row r="109" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:25">
       <c r="A109" s="7" t="s">
         <v>15</v>
       </c>
@@ -6879,7 +7043,7 @@
       <c r="U109"/>
       <c r="Y109"/>
     </row>
-    <row r="110" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:25">
       <c r="A110" s="7" t="s">
         <v>15</v>
       </c>
@@ -6913,7 +7077,7 @@
       <c r="U110"/>
       <c r="Y110"/>
     </row>
-    <row r="111" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:25">
       <c r="A111" s="7" t="s">
         <v>15</v>
       </c>
@@ -6947,7 +7111,7 @@
       <c r="U111"/>
       <c r="Y111"/>
     </row>
-    <row r="112" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:25">
       <c r="A112" s="7" t="s">
         <v>15</v>
       </c>
@@ -6987,7 +7151,7 @@
       </c>
       <c r="Y112"/>
     </row>
-    <row r="113" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:25">
       <c r="A113" s="7" t="s">
         <v>15</v>
       </c>
@@ -7033,7 +7197,7 @@
       </c>
       <c r="Y113"/>
     </row>
-    <row r="114" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:25">
       <c r="A114" s="7" t="s">
         <v>15</v>
       </c>
@@ -7091,7 +7255,7 @@
       </c>
       <c r="Y114"/>
     </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:25">
       <c r="A115" s="7" t="s">
         <v>15</v>
       </c>
@@ -7144,7 +7308,7 @@
       </c>
       <c r="Y115"/>
     </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:25">
       <c r="A116" s="7" t="s">
         <v>15</v>
       </c>
@@ -7179,7 +7343,7 @@
       <c r="U116"/>
       <c r="Y116"/>
     </row>
-    <row r="117" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:25">
       <c r="A117" s="7" t="s">
         <v>15</v>
       </c>
@@ -7214,7 +7378,7 @@
       <c r="U117"/>
       <c r="Y117"/>
     </row>
-    <row r="118" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:25">
       <c r="A118" s="7" t="s">
         <v>15</v>
       </c>
@@ -7245,7 +7409,7 @@
       <c r="U118"/>
       <c r="Y118"/>
     </row>
-    <row r="119" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:25">
       <c r="A119" s="7" t="s">
         <v>15</v>
       </c>
@@ -7287,7 +7451,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:25">
       <c r="A120" s="7" t="s">
         <v>15</v>
       </c>
@@ -7321,7 +7485,7 @@
       <c r="U120"/>
       <c r="Y120"/>
     </row>
-    <row r="121" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:25">
       <c r="A121" s="7" t="s">
         <v>15</v>
       </c>
@@ -7355,7 +7519,7 @@
       <c r="U121"/>
       <c r="Y121"/>
     </row>
-    <row r="122" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:25">
       <c r="A122" s="7" t="s">
         <v>15</v>
       </c>
@@ -7389,7 +7553,7 @@
       <c r="U122"/>
       <c r="Y122"/>
     </row>
-    <row r="123" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:25">
       <c r="A123" s="7" t="s">
         <v>15</v>
       </c>
@@ -7423,7 +7587,7 @@
       <c r="U123"/>
       <c r="Y123"/>
     </row>
-    <row r="124" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:25">
       <c r="A124" s="7" t="s">
         <v>15</v>
       </c>
@@ -7457,7 +7621,7 @@
       <c r="U124"/>
       <c r="Y124"/>
     </row>
-    <row r="125" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:25">
       <c r="A125" s="7" t="s">
         <v>15</v>
       </c>
@@ -7491,7 +7655,7 @@
       <c r="U125"/>
       <c r="Y125"/>
     </row>
-    <row r="126" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:25">
       <c r="A126" s="7" t="s">
         <v>15</v>
       </c>
@@ -7531,7 +7695,7 @@
       </c>
       <c r="Y126"/>
     </row>
-    <row r="127" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:25">
       <c r="A127" s="7" t="s">
         <v>15</v>
       </c>
@@ -7577,7 +7741,7 @@
       </c>
       <c r="Y127"/>
     </row>
-    <row r="128" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:25">
       <c r="A128" s="7" t="s">
         <v>15</v>
       </c>
@@ -7635,7 +7799,7 @@
       </c>
       <c r="Y128"/>
     </row>
-    <row r="129" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:25">
       <c r="A129" s="7" t="s">
         <v>15</v>
       </c>
@@ -7688,7 +7852,7 @@
       </c>
       <c r="Y129"/>
     </row>
-    <row r="130" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:25">
       <c r="A130" s="7" t="s">
         <v>15</v>
       </c>
@@ -7723,7 +7887,7 @@
       <c r="U130"/>
       <c r="Y130"/>
     </row>
-    <row r="131" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:25">
       <c r="A131" s="7" t="s">
         <v>15</v>
       </c>
@@ -7758,7 +7922,7 @@
       <c r="U131"/>
       <c r="Y131"/>
     </row>
-    <row r="132" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:25">
       <c r="A132" s="7" t="s">
         <v>15</v>
       </c>
@@ -7789,7 +7953,7 @@
       <c r="U132"/>
       <c r="Y132"/>
     </row>
-    <row r="133" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:25">
       <c r="A133" s="7" t="s">
         <v>15</v>
       </c>
@@ -7831,7 +7995,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="134" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:25">
       <c r="A134" s="7" t="s">
         <v>15</v>
       </c>
@@ -7865,7 +8029,7 @@
       <c r="U134"/>
       <c r="Y134"/>
     </row>
-    <row r="135" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:25">
       <c r="A135" s="7" t="s">
         <v>15</v>
       </c>
@@ -7899,7 +8063,7 @@
       <c r="U135"/>
       <c r="Y135"/>
     </row>
-    <row r="136" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:25">
       <c r="A136" s="7" t="s">
         <v>15</v>
       </c>
@@ -7933,7 +8097,7 @@
       <c r="U136"/>
       <c r="Y136"/>
     </row>
-    <row r="137" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:25">
       <c r="A137" s="7" t="s">
         <v>15</v>
       </c>
@@ -7967,7 +8131,7 @@
       <c r="U137"/>
       <c r="Y137"/>
     </row>
-    <row r="138" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:25">
       <c r="A138" s="7" t="s">
         <v>15</v>
       </c>
@@ -8001,7 +8165,7 @@
       <c r="U138"/>
       <c r="Y138"/>
     </row>
-    <row r="139" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:25">
       <c r="A139" s="7" t="s">
         <v>15</v>
       </c>
@@ -8035,7 +8199,7 @@
       <c r="U139"/>
       <c r="Y139"/>
     </row>
-    <row r="140" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:25">
       <c r="A140" s="7" t="s">
         <v>15</v>
       </c>
@@ -8067,7 +8231,7 @@
       <c r="U140"/>
       <c r="Y140"/>
     </row>
-    <row r="141" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:25">
       <c r="A141" s="7" t="s">
         <v>15</v>
       </c>
@@ -8099,7 +8263,7 @@
       <c r="N141"/>
       <c r="Y141"/>
     </row>
-    <row r="142" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:25">
       <c r="A142" s="7" t="s">
         <v>15</v>
       </c>
@@ -8155,7 +8319,7 @@
       </c>
       <c r="Y142"/>
     </row>
-    <row r="143" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:25">
       <c r="A143" s="7" t="s">
         <v>15</v>
       </c>
@@ -8208,7 +8372,7 @@
       </c>
       <c r="Y143"/>
     </row>
-    <row r="144" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:25">
       <c r="A144" s="7" t="s">
         <v>15</v>
       </c>
@@ -8261,7 +8425,7 @@
       </c>
       <c r="Y144"/>
     </row>
-    <row r="145" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:25">
       <c r="A145" s="7" t="s">
         <v>15</v>
       </c>
@@ -8312,7 +8476,7 @@
       </c>
       <c r="Y145"/>
     </row>
-    <row r="146" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:25">
       <c r="A146" s="7" t="s">
         <v>15</v>
       </c>
@@ -8353,7 +8517,7 @@
       <c r="U146"/>
       <c r="Y146"/>
     </row>
-    <row r="147" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:25">
       <c r="A147" s="7" t="s">
         <v>15</v>
       </c>
@@ -8394,7 +8558,7 @@
       <c r="U147"/>
       <c r="Y147"/>
     </row>
-    <row r="148" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:25">
       <c r="A148" s="7" t="s">
         <v>15</v>
       </c>
@@ -8433,7 +8597,7 @@
       <c r="U148"/>
       <c r="Y148"/>
     </row>
-    <row r="149" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:25">
       <c r="A149" s="7" t="s">
         <v>15</v>
       </c>
@@ -8474,7 +8638,7 @@
       <c r="T149"/>
       <c r="U149"/>
     </row>
-    <row r="150" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:25">
       <c r="A150" s="7" t="s">
         <v>15</v>
       </c>
@@ -8511,7 +8675,7 @@
       <c r="U150"/>
       <c r="Y150"/>
     </row>
-    <row r="151" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:25">
       <c r="A151" s="7" t="s">
         <v>15</v>
       </c>
@@ -8548,7 +8712,7 @@
       <c r="U151"/>
       <c r="Y151"/>
     </row>
-    <row r="152" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:25">
       <c r="A152" s="7" t="s">
         <v>15</v>
       </c>
@@ -8580,7 +8744,7 @@
       <c r="U152"/>
       <c r="Y152"/>
     </row>
-    <row r="153" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:25">
       <c r="A153" s="7" t="s">
         <v>15</v>
       </c>
@@ -8616,7 +8780,7 @@
       <c r="U153"/>
       <c r="Y153"/>
     </row>
-    <row r="154" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:25">
       <c r="A154" s="7" t="s">
         <v>15</v>
       </c>
@@ -8669,7 +8833,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="155" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:25">
       <c r="A155" s="7" t="s">
         <v>15</v>
       </c>
@@ -8717,7 +8881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:25">
       <c r="A156" s="7" t="s">
         <v>15</v>
       </c>
@@ -8745,7 +8909,7 @@
       <c r="T156"/>
       <c r="U156"/>
     </row>
-    <row r="157" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:25">
       <c r="A157" s="7" t="s">
         <v>15</v>
       </c>
@@ -8773,7 +8937,7 @@
       <c r="T157"/>
       <c r="U157"/>
     </row>
-    <row r="158" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:25">
       <c r="A158" s="7" t="s">
         <v>15</v>
       </c>
@@ -8799,7 +8963,7 @@
       <c r="T158"/>
       <c r="U158"/>
     </row>
-    <row r="159" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:25">
       <c r="A159" s="7" t="s">
         <v>15</v>
       </c>
@@ -8825,7 +8989,7 @@
       <c r="T159"/>
       <c r="U159"/>
     </row>
-    <row r="160" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:25">
       <c r="A160" s="7" t="s">
         <v>15</v>
       </c>
@@ -8854,7 +9018,7 @@
       <c r="T160"/>
       <c r="U160"/>
     </row>
-    <row r="161" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:25">
       <c r="A161" s="7" t="s">
         <v>15</v>
       </c>
@@ -8879,7 +9043,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="162" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:25">
       <c r="A162" s="7" t="s">
         <v>15</v>
       </c>
@@ -8904,7 +9068,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="163" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:25">
       <c r="A163" s="7" t="s">
         <v>15</v>
       </c>
@@ -8932,7 +9096,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="164" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:25">
       <c r="A164" s="7" t="s">
         <v>15</v>
       </c>
@@ -8960,7 +9124,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="165" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:25">
       <c r="A165" s="7" t="s">
         <v>15</v>
       </c>
@@ -8988,7 +9152,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="166" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:25">
       <c r="A166" s="7" t="s">
         <v>312</v>
       </c>
@@ -9020,7 +9184,7 @@
       <c r="U166"/>
       <c r="Y166"/>
     </row>
-    <row r="167" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:25">
       <c r="A167" s="7" t="s">
         <v>15</v>
       </c>
@@ -9056,7 +9220,7 @@
       <c r="U167"/>
       <c r="Y167"/>
     </row>
-    <row r="168" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:25">
       <c r="A168" s="7" t="s">
         <v>15</v>
       </c>
@@ -9109,7 +9273,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="169" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:25">
       <c r="A169" s="7" t="s">
         <v>15</v>
       </c>
@@ -9157,7 +9321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:25">
       <c r="A170" s="7" t="s">
         <v>15</v>
       </c>
@@ -9185,7 +9349,7 @@
       <c r="T170"/>
       <c r="U170"/>
     </row>
-    <row r="171" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:25">
       <c r="A171" s="7" t="s">
         <v>15</v>
       </c>
@@ -9213,7 +9377,7 @@
       <c r="T171"/>
       <c r="U171"/>
     </row>
-    <row r="172" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:25">
       <c r="A172" s="7" t="s">
         <v>15</v>
       </c>
@@ -9239,7 +9403,7 @@
       <c r="T172"/>
       <c r="U172"/>
     </row>
-    <row r="173" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:25">
       <c r="A173" s="7" t="s">
         <v>15</v>
       </c>
@@ -9265,7 +9429,7 @@
       <c r="T173"/>
       <c r="U173"/>
     </row>
-    <row r="174" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:25">
       <c r="A174" s="7" t="s">
         <v>15</v>
       </c>
@@ -9294,7 +9458,7 @@
       <c r="T174"/>
       <c r="U174"/>
     </row>
-    <row r="175" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:25">
       <c r="A175" s="7" t="s">
         <v>15</v>
       </c>
@@ -9319,7 +9483,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="176" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:25">
       <c r="A176" s="7" t="s">
         <v>15</v>
       </c>
@@ -9344,7 +9508,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="177" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:25">
       <c r="A177" s="7" t="s">
         <v>15</v>
       </c>
@@ -9372,7 +9536,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="178" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:25">
       <c r="A178" s="7" t="s">
         <v>15</v>
       </c>
@@ -9400,7 +9564,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="179" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:25">
       <c r="A179" s="7" t="s">
         <v>15</v>
       </c>
@@ -9428,7 +9592,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="180" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:25">
       <c r="A180" s="7" t="s">
         <v>312</v>
       </c>
@@ -9460,7 +9624,7 @@
       <c r="U180"/>
       <c r="Y180"/>
     </row>
-    <row r="181" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:25">
       <c r="A181" s="7" t="s">
         <v>15</v>
       </c>
@@ -9496,7 +9660,7 @@
       <c r="U181"/>
       <c r="Y181"/>
     </row>
-    <row r="182" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:25">
       <c r="A182" s="7" t="s">
         <v>15</v>
       </c>
@@ -9554,7 +9718,7 @@
       </c>
       <c r="Y182"/>
     </row>
-    <row r="183" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:25">
       <c r="A183" s="7" t="s">
         <v>15</v>
       </c>
@@ -9607,7 +9771,7 @@
       </c>
       <c r="Y183"/>
     </row>
-    <row r="184" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:25">
       <c r="A184" s="7" t="s">
         <v>15</v>
       </c>
@@ -9642,7 +9806,7 @@
       <c r="U184"/>
       <c r="Y184"/>
     </row>
-    <row r="185" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:25">
       <c r="A185" s="7" t="s">
         <v>15</v>
       </c>
@@ -9677,7 +9841,7 @@
       <c r="U185"/>
       <c r="Y185"/>
     </row>
-    <row r="186" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:25">
       <c r="A186" s="7" t="s">
         <v>15</v>
       </c>
@@ -9708,7 +9872,7 @@
       <c r="U186"/>
       <c r="Y186"/>
     </row>
-    <row r="187" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:25">
       <c r="A187" s="7" t="s">
         <v>15</v>
       </c>
@@ -9738,7 +9902,7 @@
       <c r="T187"/>
       <c r="U187"/>
     </row>
-    <row r="188" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:25">
       <c r="A188" s="7" t="s">
         <v>15</v>
       </c>
@@ -9772,7 +9936,7 @@
       <c r="U188"/>
       <c r="Y188"/>
     </row>
-    <row r="189" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:25">
       <c r="A189" s="7" t="s">
         <v>15</v>
       </c>
@@ -9802,7 +9966,7 @@
       <c r="N189" s="15"/>
       <c r="Y189"/>
     </row>
-    <row r="190" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:25">
       <c r="A190" s="7" t="s">
         <v>15</v>
       </c>
@@ -9832,7 +9996,7 @@
       <c r="N190" s="15"/>
       <c r="Y190"/>
     </row>
-    <row r="191" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:25">
       <c r="A191" s="7" t="s">
         <v>15</v>
       </c>
@@ -9865,7 +10029,7 @@
       </c>
       <c r="Y191"/>
     </row>
-    <row r="192" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:25">
       <c r="A192" s="7" t="s">
         <v>15</v>
       </c>
@@ -9898,7 +10062,7 @@
       </c>
       <c r="Y192"/>
     </row>
-    <row r="193" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:25">
       <c r="A193" s="7" t="s">
         <v>15</v>
       </c>
@@ -9931,7 +10095,7 @@
       </c>
       <c r="Y193"/>
     </row>
-    <row r="194" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:25">
       <c r="A194" s="7" t="s">
         <v>312</v>
       </c>
@@ -9963,7 +10127,7 @@
       <c r="U194"/>
       <c r="Y194"/>
     </row>
-    <row r="195" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:25">
       <c r="A195" s="7" t="s">
         <v>15</v>
       </c>
@@ -9999,7 +10163,7 @@
       <c r="U195"/>
       <c r="Y195"/>
     </row>
-    <row r="196" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:25">
       <c r="A196" s="7" t="s">
         <v>15</v>
       </c>
@@ -10052,7 +10216,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="197" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:25">
       <c r="A197" s="7" t="s">
         <v>15</v>
       </c>
@@ -10100,7 +10264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:25">
       <c r="A198" s="7" t="s">
         <v>15</v>
       </c>
@@ -10128,7 +10292,7 @@
       <c r="T198"/>
       <c r="U198"/>
     </row>
-    <row r="199" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:25">
       <c r="A199" s="7" t="s">
         <v>15</v>
       </c>
@@ -10156,7 +10320,7 @@
       <c r="T199"/>
       <c r="U199"/>
     </row>
-    <row r="200" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:25">
       <c r="A200" s="7" t="s">
         <v>15</v>
       </c>
@@ -10182,7 +10346,7 @@
       <c r="T200"/>
       <c r="U200"/>
     </row>
-    <row r="201" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:25">
       <c r="A201" s="7" t="s">
         <v>15</v>
       </c>
@@ -10208,7 +10372,7 @@
       <c r="T201"/>
       <c r="U201"/>
     </row>
-    <row r="202" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:25">
       <c r="A202" s="7" t="s">
         <v>15</v>
       </c>
@@ -10237,7 +10401,7 @@
       <c r="T202"/>
       <c r="U202"/>
     </row>
-    <row r="203" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:25">
       <c r="A203" s="7" t="s">
         <v>15</v>
       </c>
@@ -10262,7 +10426,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="204" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:25">
       <c r="A204" s="7" t="s">
         <v>15</v>
       </c>
@@ -10287,7 +10451,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="205" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:25">
       <c r="A205" s="7" t="s">
         <v>15</v>
       </c>
@@ -10315,7 +10479,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="206" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:25">
       <c r="A206" s="7" t="s">
         <v>15</v>
       </c>
@@ -10343,7 +10507,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="207" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:25">
       <c r="A207" s="7" t="s">
         <v>15</v>
       </c>
@@ -10371,7 +10535,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="208" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:25">
       <c r="A208" s="7" t="s">
         <v>15</v>
       </c>
@@ -10403,7 +10567,7 @@
       <c r="U208"/>
       <c r="Y208"/>
     </row>
-    <row r="209" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:25">
       <c r="A209" s="7" t="s">
         <v>15</v>
       </c>
@@ -10439,7 +10603,7 @@
       <c r="U209"/>
       <c r="Y209"/>
     </row>
-    <row r="210" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:25">
       <c r="A210" s="7" t="s">
         <v>15</v>
       </c>
@@ -10497,7 +10661,7 @@
       </c>
       <c r="Y210"/>
     </row>
-    <row r="211" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:25">
       <c r="A211" s="7" t="s">
         <v>15</v>
       </c>
@@ -10550,7 +10714,7 @@
       </c>
       <c r="Y211"/>
     </row>
-    <row r="212" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:25">
       <c r="A212" s="7" t="s">
         <v>15</v>
       </c>
@@ -10583,7 +10747,7 @@
       <c r="U212"/>
       <c r="Y212"/>
     </row>
-    <row r="213" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:25">
       <c r="A213" s="7" t="s">
         <v>15</v>
       </c>
@@ -10614,7 +10778,7 @@
       <c r="U213"/>
       <c r="Y213"/>
     </row>
-    <row r="214" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:25">
       <c r="A214" s="7" t="s">
         <v>15</v>
       </c>
@@ -10649,7 +10813,7 @@
       <c r="U214"/>
       <c r="Y214"/>
     </row>
-    <row r="215" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:25">
       <c r="A215" s="7" t="s">
         <v>15</v>
       </c>
@@ -10684,7 +10848,7 @@
       <c r="U215"/>
       <c r="Y215"/>
     </row>
-    <row r="216" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:25">
       <c r="A216" s="7" t="s">
         <v>15</v>
       </c>
@@ -10718,7 +10882,7 @@
       <c r="U216"/>
       <c r="Y216"/>
     </row>
-    <row r="217" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:25">
       <c r="A217" s="7" t="s">
         <v>15</v>
       </c>
@@ -10750,7 +10914,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="218" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:25">
       <c r="A218" s="7" t="s">
         <v>15</v>
       </c>
@@ -10783,7 +10947,7 @@
       </c>
       <c r="Y218"/>
     </row>
-    <row r="219" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:25">
       <c r="A219" s="7" t="s">
         <v>15</v>
       </c>
@@ -10816,7 +10980,7 @@
       </c>
       <c r="Y219"/>
     </row>
-    <row r="220" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:25">
       <c r="A220" s="7" t="s">
         <v>312</v>
       </c>
@@ -10848,7 +11012,7 @@
       <c r="U220"/>
       <c r="Y220"/>
     </row>
-    <row r="221" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:25">
       <c r="A221" s="7" t="s">
         <v>15</v>
       </c>
@@ -10884,7 +11048,7 @@
       <c r="U221"/>
       <c r="Y221"/>
     </row>
-    <row r="222" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:25">
       <c r="A222" s="7" t="s">
         <v>15</v>
       </c>
@@ -10942,7 +11106,7 @@
       </c>
       <c r="Y222"/>
     </row>
-    <row r="223" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:25">
       <c r="A223" s="7" t="s">
         <v>15</v>
       </c>
@@ -10995,7 +11159,7 @@
       </c>
       <c r="Y223"/>
     </row>
-    <row r="224" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:25">
       <c r="A224" s="7" t="s">
         <v>15</v>
       </c>
@@ -11028,7 +11192,7 @@
       <c r="U224"/>
       <c r="Y224"/>
     </row>
-    <row r="225" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:25">
       <c r="A225" s="7" t="s">
         <v>15</v>
       </c>
@@ -11059,7 +11223,7 @@
       <c r="U225"/>
       <c r="Y225"/>
     </row>
-    <row r="226" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:25">
       <c r="A226" s="7" t="s">
         <v>15</v>
       </c>
@@ -11094,7 +11258,7 @@
       <c r="U226"/>
       <c r="Y226"/>
     </row>
-    <row r="227" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:25">
       <c r="A227" s="7" t="s">
         <v>15</v>
       </c>
@@ -11129,7 +11293,7 @@
       <c r="U227"/>
       <c r="Y227"/>
     </row>
-    <row r="228" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:25">
       <c r="A228" s="7" t="s">
         <v>15</v>
       </c>
@@ -11163,7 +11327,7 @@
       <c r="U228"/>
       <c r="Y228"/>
     </row>
-    <row r="229" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:25">
       <c r="A229" s="7" t="s">
         <v>15</v>
       </c>
@@ -11195,7 +11359,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="230" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:25">
       <c r="A230" s="7" t="s">
         <v>15</v>
       </c>
@@ -11228,7 +11392,7 @@
       </c>
       <c r="Y230"/>
     </row>
-    <row r="231" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:25">
       <c r="A231" s="7" t="s">
         <v>15</v>
       </c>
@@ -11261,7 +11425,7 @@
       </c>
       <c r="Y231"/>
     </row>
-    <row r="232" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:25">
       <c r="A232" s="7" t="s">
         <v>312</v>
       </c>
@@ -11293,7 +11457,7 @@
       <c r="U232"/>
       <c r="Y232"/>
     </row>
-    <row r="233" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:25">
       <c r="A233" s="7" t="s">
         <v>15</v>
       </c>
@@ -11329,7 +11493,7 @@
       <c r="U233"/>
       <c r="Y233"/>
     </row>
-    <row r="234" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:25">
       <c r="A234" s="7" t="s">
         <v>15</v>
       </c>
@@ -11387,7 +11551,7 @@
       </c>
       <c r="Y234"/>
     </row>
-    <row r="235" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:25">
       <c r="A235" s="7" t="s">
         <v>15</v>
       </c>
@@ -11440,7 +11604,7 @@
       </c>
       <c r="Y235"/>
     </row>
-    <row r="236" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:25">
       <c r="A236" s="7" t="s">
         <v>15</v>
       </c>
@@ -11473,7 +11637,7 @@
       <c r="U236"/>
       <c r="Y236"/>
     </row>
-    <row r="237" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:25">
       <c r="A237" s="7" t="s">
         <v>15</v>
       </c>
@@ -11504,7 +11668,7 @@
       <c r="U237"/>
       <c r="Y237"/>
     </row>
-    <row r="238" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:25">
       <c r="A238" s="7" t="s">
         <v>15</v>
       </c>
@@ -11539,7 +11703,7 @@
       <c r="U238"/>
       <c r="Y238"/>
     </row>
-    <row r="239" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:25">
       <c r="A239" s="7" t="s">
         <v>15</v>
       </c>
@@ -11574,7 +11738,7 @@
       <c r="U239"/>
       <c r="Y239"/>
     </row>
-    <row r="240" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:25">
       <c r="A240" s="7" t="s">
         <v>15</v>
       </c>
@@ -11608,7 +11772,7 @@
       <c r="U240"/>
       <c r="Y240"/>
     </row>
-    <row r="241" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:25">
       <c r="A241" s="7" t="s">
         <v>15</v>
       </c>
@@ -11640,7 +11804,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="242" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:25">
       <c r="A242" s="7" t="s">
         <v>15</v>
       </c>
@@ -11673,7 +11837,7 @@
       </c>
       <c r="Y242"/>
     </row>
-    <row r="243" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:25">
       <c r="A243" s="7" t="s">
         <v>15</v>
       </c>
@@ -11706,7 +11870,7 @@
       </c>
       <c r="Y243"/>
     </row>
-    <row r="244" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:25">
       <c r="A244" s="7" t="s">
         <v>312</v>
       </c>
@@ -11738,7 +11902,7 @@
       <c r="U244"/>
       <c r="Y244"/>
     </row>
-    <row r="245" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:25">
       <c r="A245" s="7" t="s">
         <v>15</v>
       </c>
@@ -11774,7 +11938,7 @@
       <c r="U245"/>
       <c r="Y245"/>
     </row>
-    <row r="246" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:25">
       <c r="A246" s="7" t="s">
         <v>15</v>
       </c>
@@ -11832,7 +11996,7 @@
       </c>
       <c r="Y246"/>
     </row>
-    <row r="247" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:25">
       <c r="A247" s="7" t="s">
         <v>15</v>
       </c>
@@ -11885,7 +12049,7 @@
       </c>
       <c r="Y247"/>
     </row>
-    <row r="248" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:25">
       <c r="A248" s="7" t="s">
         <v>15</v>
       </c>
@@ -11918,7 +12082,7 @@
       <c r="U248"/>
       <c r="Y248"/>
     </row>
-    <row r="249" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:25">
       <c r="A249" s="7" t="s">
         <v>15</v>
       </c>
@@ -11949,7 +12113,7 @@
       <c r="U249"/>
       <c r="Y249"/>
     </row>
-    <row r="250" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:25">
       <c r="A250" s="7" t="s">
         <v>15</v>
       </c>
@@ -11984,7 +12148,7 @@
       <c r="U250"/>
       <c r="Y250"/>
     </row>
-    <row r="251" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:25">
       <c r="A251" s="7" t="s">
         <v>15</v>
       </c>
@@ -12019,7 +12183,7 @@
       <c r="U251"/>
       <c r="Y251"/>
     </row>
-    <row r="252" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:25">
       <c r="A252" s="7" t="s">
         <v>15</v>
       </c>
@@ -12053,7 +12217,7 @@
       <c r="U252"/>
       <c r="Y252"/>
     </row>
-    <row r="253" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:25">
       <c r="A253" s="7" t="s">
         <v>15</v>
       </c>
@@ -12085,7 +12249,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="254" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:25">
       <c r="A254" s="7" t="s">
         <v>15</v>
       </c>
@@ -12118,7 +12282,7 @@
       </c>
       <c r="Y254"/>
     </row>
-    <row r="255" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:25">
       <c r="A255" s="7" t="s">
         <v>15</v>
       </c>
@@ -12151,7 +12315,7 @@
       </c>
       <c r="Y255"/>
     </row>
-    <row r="256" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:25">
       <c r="A256" s="7" t="s">
         <v>312</v>
       </c>
@@ -12183,7 +12347,7 @@
       <c r="U256"/>
       <c r="Y256"/>
     </row>
-    <row r="257" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:25">
       <c r="A257" s="7" t="s">
         <v>15</v>
       </c>
@@ -12219,7 +12383,7 @@
       <c r="U257"/>
       <c r="Y257"/>
     </row>
-    <row r="258" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:25">
       <c r="A258" s="7" t="s">
         <v>15</v>
       </c>
@@ -12277,7 +12441,7 @@
       </c>
       <c r="Y258"/>
     </row>
-    <row r="259" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:25">
       <c r="A259" s="7" t="s">
         <v>15</v>
       </c>
@@ -12330,7 +12494,7 @@
       </c>
       <c r="Y259"/>
     </row>
-    <row r="260" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:25">
       <c r="A260" s="7" t="s">
         <v>15</v>
       </c>
@@ -12363,7 +12527,7 @@
       <c r="U260"/>
       <c r="Y260"/>
     </row>
-    <row r="261" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:25">
       <c r="A261" s="7" t="s">
         <v>15</v>
       </c>
@@ -12394,7 +12558,7 @@
       <c r="U261"/>
       <c r="Y261"/>
     </row>
-    <row r="262" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:25">
       <c r="A262" s="7" t="s">
         <v>15</v>
       </c>
@@ -12429,7 +12593,7 @@
       <c r="U262"/>
       <c r="Y262"/>
     </row>
-    <row r="263" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:25">
       <c r="A263" s="7" t="s">
         <v>15</v>
       </c>
@@ -12464,7 +12628,7 @@
       <c r="U263"/>
       <c r="Y263"/>
     </row>
-    <row r="264" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:25">
       <c r="A264" s="7" t="s">
         <v>15</v>
       </c>
@@ -12498,7 +12662,7 @@
       <c r="U264"/>
       <c r="Y264"/>
     </row>
-    <row r="265" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:25">
       <c r="A265" s="7" t="s">
         <v>15</v>
       </c>
@@ -12530,7 +12694,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="266" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:25">
       <c r="A266" s="7" t="s">
         <v>15</v>
       </c>
@@ -12563,7 +12727,7 @@
       </c>
       <c r="Y266"/>
     </row>
-    <row r="267" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:25">
       <c r="A267" s="7" t="s">
         <v>15</v>
       </c>
@@ -12596,7 +12760,7 @@
       </c>
       <c r="Y267"/>
     </row>
-    <row r="268" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:25">
       <c r="A268" s="7" t="s">
         <v>312</v>
       </c>
@@ -12628,7 +12792,7 @@
       <c r="U268"/>
       <c r="Y268"/>
     </row>
-    <row r="269" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:25">
       <c r="A269" s="7" t="s">
         <v>15</v>
       </c>
@@ -12664,7 +12828,7 @@
       <c r="U269"/>
       <c r="Y269"/>
     </row>
-    <row r="270" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:25">
       <c r="A270" s="7" t="s">
         <v>15</v>
       </c>
@@ -12700,7 +12864,7 @@
       <c r="U270"/>
       <c r="Y270"/>
     </row>
-    <row r="271" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:25">
       <c r="A271" s="7" t="s">
         <v>15</v>
       </c>
@@ -12756,7 +12920,7 @@
       </c>
       <c r="Y271"/>
     </row>
-    <row r="272" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:25">
       <c r="A272" s="7" t="s">
         <v>15</v>
       </c>
@@ -12809,7 +12973,7 @@
       </c>
       <c r="Y272"/>
     </row>
-    <row r="273" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:25">
       <c r="A273" s="7" t="s">
         <v>15</v>
       </c>
@@ -12840,7 +13004,7 @@
       <c r="U273"/>
       <c r="Y273"/>
     </row>
-    <row r="274" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:25">
       <c r="A274" s="7" t="s">
         <v>15</v>
       </c>
@@ -12875,7 +13039,7 @@
       <c r="U274"/>
       <c r="Y274"/>
     </row>
-    <row r="275" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:25">
       <c r="A275" s="7" t="s">
         <v>15</v>
       </c>
@@ -12910,7 +13074,7 @@
       <c r="U275"/>
       <c r="Y275"/>
     </row>
-    <row r="276" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:25">
       <c r="A276" s="7" t="s">
         <v>15</v>
       </c>
@@ -12943,7 +13107,7 @@
       <c r="U276"/>
       <c r="Y276"/>
     </row>
-    <row r="277" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:25">
       <c r="A277" s="7" t="s">
         <v>15</v>
       </c>
@@ -12976,7 +13140,7 @@
       <c r="T277"/>
       <c r="U277"/>
     </row>
-    <row r="278" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:25">
       <c r="A278" s="7" t="s">
         <v>15</v>
       </c>
@@ -13009,7 +13173,7 @@
       </c>
       <c r="Y278"/>
     </row>
-    <row r="279" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:25">
       <c r="A279" s="7" t="s">
         <v>15</v>
       </c>
@@ -13042,7 +13206,7 @@
       </c>
       <c r="Y279"/>
     </row>
-    <row r="280" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:25">
       <c r="A280" s="7" t="s">
         <v>312</v>
       </c>
@@ -13074,7 +13238,7 @@
       <c r="U280"/>
       <c r="Y280"/>
     </row>
-    <row r="281" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:25">
       <c r="A281" s="7" t="s">
         <v>15</v>
       </c>
@@ -13110,7 +13274,7 @@
       <c r="U281"/>
       <c r="Y281"/>
     </row>
-    <row r="282" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:25">
       <c r="A282" s="7" t="s">
         <v>15</v>
       </c>
@@ -13168,7 +13332,7 @@
       </c>
       <c r="Y282"/>
     </row>
-    <row r="283" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:25">
       <c r="A283" s="7" t="s">
         <v>15</v>
       </c>
@@ -13221,7 +13385,7 @@
       </c>
       <c r="Y283"/>
     </row>
-    <row r="284" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:25">
       <c r="A284" s="7" t="s">
         <v>15</v>
       </c>
@@ -13254,7 +13418,7 @@
       <c r="U284"/>
       <c r="Y284"/>
     </row>
-    <row r="285" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:25">
       <c r="A285" s="7" t="s">
         <v>15</v>
       </c>
@@ -13285,7 +13449,7 @@
       <c r="U285"/>
       <c r="Y285"/>
     </row>
-    <row r="286" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:25">
       <c r="A286" s="7" t="s">
         <v>15</v>
       </c>
@@ -13320,7 +13484,7 @@
       <c r="U286"/>
       <c r="Y286"/>
     </row>
-    <row r="287" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:25">
       <c r="A287" s="7" t="s">
         <v>15</v>
       </c>
@@ -13355,7 +13519,7 @@
       <c r="U287"/>
       <c r="Y287"/>
     </row>
-    <row r="288" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:25">
       <c r="A288" s="7" t="s">
         <v>15</v>
       </c>
@@ -13389,7 +13553,7 @@
       <c r="U288"/>
       <c r="Y288"/>
     </row>
-    <row r="289" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:25">
       <c r="A289" s="7" t="s">
         <v>15</v>
       </c>
@@ -13421,7 +13585,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="290" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:25">
       <c r="A290" s="7" t="s">
         <v>15</v>
       </c>
@@ -13454,7 +13618,7 @@
       </c>
       <c r="Y290"/>
     </row>
-    <row r="291" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:25">
       <c r="A291" s="7" t="s">
         <v>15</v>
       </c>
@@ -13487,7 +13651,7 @@
       </c>
       <c r="Y291"/>
     </row>
-    <row r="292" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:25">
       <c r="A292" s="7" t="s">
         <v>312</v>
       </c>
@@ -13519,7 +13683,7 @@
       <c r="U292"/>
       <c r="Y292"/>
     </row>
-    <row r="293" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:25">
       <c r="A293" s="7" t="s">
         <v>15</v>
       </c>
@@ -13555,7 +13719,7 @@
       <c r="U293"/>
       <c r="Y293"/>
     </row>
-    <row r="294" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:25">
       <c r="A294" s="7" t="s">
         <v>15</v>
       </c>
@@ -13613,7 +13777,7 @@
       </c>
       <c r="Y294"/>
     </row>
-    <row r="295" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:25">
       <c r="A295" s="7" t="s">
         <v>15</v>
       </c>
@@ -13666,7 +13830,7 @@
       </c>
       <c r="Y295"/>
     </row>
-    <row r="296" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:25">
       <c r="A296" s="7" t="s">
         <v>15</v>
       </c>
@@ -13699,7 +13863,7 @@
       <c r="U296"/>
       <c r="Y296"/>
     </row>
-    <row r="297" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:25">
       <c r="A297" s="7" t="s">
         <v>15</v>
       </c>
@@ -13730,7 +13894,7 @@
       <c r="U297"/>
       <c r="Y297"/>
     </row>
-    <row r="298" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:25">
       <c r="A298" s="7" t="s">
         <v>15</v>
       </c>
@@ -13765,7 +13929,7 @@
       <c r="U298"/>
       <c r="Y298"/>
     </row>
-    <row r="299" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:25">
       <c r="A299" s="7" t="s">
         <v>15</v>
       </c>
@@ -13800,7 +13964,7 @@
       <c r="U299"/>
       <c r="Y299"/>
     </row>
-    <row r="300" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:25">
       <c r="A300" s="7" t="s">
         <v>15</v>
       </c>
@@ -13834,7 +13998,7 @@
       <c r="U300"/>
       <c r="Y300"/>
     </row>
-    <row r="301" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:25">
       <c r="A301" s="7" t="s">
         <v>15</v>
       </c>
@@ -13866,7 +14030,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="302" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:25">
       <c r="A302" s="7" t="s">
         <v>15</v>
       </c>
@@ -13899,7 +14063,7 @@
       </c>
       <c r="Y302"/>
     </row>
-    <row r="303" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:25">
       <c r="A303" s="7" t="s">
         <v>15</v>
       </c>
@@ -13932,7 +14096,7 @@
       </c>
       <c r="Y303"/>
     </row>
-    <row r="304" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:25">
       <c r="A304" s="7" t="s">
         <v>312</v>
       </c>
@@ -13964,7 +14128,7 @@
       <c r="U304"/>
       <c r="Y304"/>
     </row>
-    <row r="305" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:25">
       <c r="A305" s="7" t="s">
         <v>15</v>
       </c>
@@ -14000,7 +14164,7 @@
       <c r="U305"/>
       <c r="Y305"/>
     </row>
-    <row r="306" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:25">
       <c r="A306" s="7" t="s">
         <v>15</v>
       </c>
@@ -14058,7 +14222,7 @@
       </c>
       <c r="Y306"/>
     </row>
-    <row r="307" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:25">
       <c r="A307" s="7" t="s">
         <v>15</v>
       </c>
@@ -14111,7 +14275,7 @@
       </c>
       <c r="Y307"/>
     </row>
-    <row r="308" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:25">
       <c r="A308" s="7" t="s">
         <v>15</v>
       </c>
@@ -14144,7 +14308,7 @@
       <c r="U308"/>
       <c r="Y308"/>
     </row>
-    <row r="309" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:25">
       <c r="A309" s="7" t="s">
         <v>15</v>
       </c>
@@ -14175,7 +14339,7 @@
       <c r="U309"/>
       <c r="Y309"/>
     </row>
-    <row r="310" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:25">
       <c r="A310" s="7" t="s">
         <v>15</v>
       </c>
@@ -14210,7 +14374,7 @@
       <c r="U310"/>
       <c r="Y310"/>
     </row>
-    <row r="311" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:25">
       <c r="A311" s="7" t="s">
         <v>15</v>
       </c>
@@ -14245,7 +14409,7 @@
       <c r="U311"/>
       <c r="Y311"/>
     </row>
-    <row r="312" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:25">
       <c r="A312" s="7" t="s">
         <v>15</v>
       </c>
@@ -14279,7 +14443,7 @@
       <c r="U312"/>
       <c r="Y312"/>
     </row>
-    <row r="313" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:25">
       <c r="A313" s="7" t="s">
         <v>15</v>
       </c>
@@ -14311,7 +14475,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="314" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:25">
       <c r="A314" s="7" t="s">
         <v>15</v>
       </c>
@@ -14344,7 +14508,7 @@
       </c>
       <c r="Y314"/>
     </row>
-    <row r="315" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:25">
       <c r="A315" s="7" t="s">
         <v>15</v>
       </c>
@@ -14377,7 +14541,7 @@
       </c>
       <c r="Y315"/>
     </row>
-    <row r="316" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:25">
       <c r="A316" s="7" t="s">
         <v>312</v>
       </c>
@@ -14409,7 +14573,7 @@
       <c r="U316"/>
       <c r="Y316"/>
     </row>
-    <row r="317" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:25">
       <c r="A317" s="7" t="s">
         <v>15</v>
       </c>
@@ -14445,7 +14609,7 @@
       <c r="U317"/>
       <c r="Y317"/>
     </row>
-    <row r="318" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:25">
       <c r="A318" s="7" t="s">
         <v>15</v>
       </c>
@@ -14503,7 +14667,7 @@
       </c>
       <c r="Y318"/>
     </row>
-    <row r="319" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:25">
       <c r="A319" s="7" t="s">
         <v>15</v>
       </c>
@@ -14556,7 +14720,7 @@
       </c>
       <c r="Y319"/>
     </row>
-    <row r="320" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:25">
       <c r="A320" s="7" t="s">
         <v>15</v>
       </c>
@@ -14589,7 +14753,7 @@
       <c r="U320"/>
       <c r="Y320"/>
     </row>
-    <row r="321" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:25">
       <c r="A321" s="7" t="s">
         <v>15</v>
       </c>
@@ -14620,7 +14784,7 @@
       <c r="U321"/>
       <c r="Y321"/>
     </row>
-    <row r="322" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:25">
       <c r="A322" s="7" t="s">
         <v>15</v>
       </c>
@@ -14655,7 +14819,7 @@
       <c r="U322"/>
       <c r="Y322"/>
     </row>
-    <row r="323" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:25">
       <c r="A323" s="7" t="s">
         <v>15</v>
       </c>
@@ -14690,7 +14854,7 @@
       <c r="U323"/>
       <c r="Y323"/>
     </row>
-    <row r="324" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:25">
       <c r="A324" s="7" t="s">
         <v>15</v>
       </c>
@@ -14724,7 +14888,7 @@
       <c r="U324"/>
       <c r="Y324"/>
     </row>
-    <row r="325" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:25">
       <c r="A325" s="7" t="s">
         <v>15</v>
       </c>
@@ -14756,7 +14920,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="326" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:25">
       <c r="A326" s="7" t="s">
         <v>15</v>
       </c>
@@ -14789,7 +14953,7 @@
       </c>
       <c r="Y326"/>
     </row>
-    <row r="327" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:25">
       <c r="A327" s="7" t="s">
         <v>15</v>
       </c>
@@ -14822,7 +14986,7 @@
       </c>
       <c r="Y327"/>
     </row>
-    <row r="328" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:25">
       <c r="A328" s="7" t="s">
         <v>312</v>
       </c>
@@ -14854,7 +15018,7 @@
       <c r="U328"/>
       <c r="Y328"/>
     </row>
-    <row r="329" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:25">
       <c r="A329" s="7" t="s">
         <v>15</v>
       </c>
@@ -14890,7 +15054,7 @@
       <c r="U329"/>
       <c r="Y329"/>
     </row>
-    <row r="330" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:25">
       <c r="A330" s="7" t="s">
         <v>15</v>
       </c>
@@ -14948,7 +15112,7 @@
       </c>
       <c r="Y330"/>
     </row>
-    <row r="331" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:25">
       <c r="A331" s="7" t="s">
         <v>15</v>
       </c>
@@ -15001,7 +15165,7 @@
       </c>
       <c r="Y331"/>
     </row>
-    <row r="332" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:25">
       <c r="A332" s="7" t="s">
         <v>15</v>
       </c>
@@ -15043,7 +15207,7 @@
       </c>
       <c r="Y332"/>
     </row>
-    <row r="333" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:25">
       <c r="A333" s="7" t="s">
         <v>15</v>
       </c>
@@ -15074,7 +15238,7 @@
       <c r="U333"/>
       <c r="Y333"/>
     </row>
-    <row r="334" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:25">
       <c r="A334" s="7" t="s">
         <v>15</v>
       </c>
@@ -15109,7 +15273,7 @@
       <c r="U334"/>
       <c r="Y334"/>
     </row>
-    <row r="335" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:25">
       <c r="A335" s="7" t="s">
         <v>15</v>
       </c>
@@ -15144,7 +15308,7 @@
       <c r="U335"/>
       <c r="Y335"/>
     </row>
-    <row r="336" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:25">
       <c r="A336" s="7" t="s">
         <v>15</v>
       </c>
@@ -15178,7 +15342,7 @@
       <c r="U336"/>
       <c r="Y336"/>
     </row>
-    <row r="337" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:25">
       <c r="A337" s="7" t="s">
         <v>15</v>
       </c>
@@ -15210,7 +15374,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="338" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:25">
       <c r="A338" s="7" t="s">
         <v>15</v>
       </c>
@@ -15243,7 +15407,7 @@
       </c>
       <c r="Y338"/>
     </row>
-    <row r="339" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:25">
       <c r="A339" s="7" t="s">
         <v>15</v>
       </c>
@@ -15292,7 +15456,7 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.2"/>
   <cols>
     <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.77734375" bestFit="1" customWidth="1"/>
@@ -15300,7 +15464,7 @@
     <col min="4" max="4" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" s="18" t="s">
         <v>246</v>
       </c>
@@ -15308,7 +15472,7 @@
       <c r="C1" s="18"/>
       <c r="D1" s="18"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" s="18" t="s">
         <v>247</v>
       </c>
@@ -15322,7 +15486,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" s="19" t="s">
         <v>67</v>
       </c>
@@ -15336,7 +15500,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" s="19" t="s">
         <v>67</v>
       </c>
@@ -15350,7 +15514,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="A5" s="19" t="s">
         <v>67</v>
       </c>
@@ -15364,7 +15528,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="A6" s="19" t="s">
         <v>67</v>
       </c>
@@ -15378,7 +15542,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="19" t="s">
         <v>67</v>
       </c>
@@ -15392,7 +15556,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="19" t="s">
         <v>67</v>
       </c>
@@ -15404,7 +15568,7 @@
       </c>
       <c r="D8" s="20"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="19" t="s">
         <v>36</v>
       </c>
@@ -15418,7 +15582,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="19" t="s">
         <v>36</v>
       </c>
@@ -15432,7 +15596,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4">
       <c r="A11" s="19" t="s">
         <v>38</v>
       </c>
@@ -15446,7 +15610,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="A12" s="19" t="s">
         <v>37</v>
       </c>
@@ -15458,7 +15622,7 @@
       </c>
       <c r="D12" s="20"/>
     </row>
-    <row r="13" spans="1:4" ht="32.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="32.4">
       <c r="A13" s="19" t="s">
         <v>35</v>
       </c>
@@ -15472,7 +15636,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="32.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="32.4">
       <c r="A14" s="19" t="s">
         <v>35</v>
       </c>
@@ -15486,7 +15650,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="32.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="32.4">
       <c r="A15" s="19" t="s">
         <v>35</v>
       </c>
@@ -15500,7 +15664,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="A16" s="19" t="s">
         <v>34</v>
       </c>
@@ -15512,7 +15676,7 @@
       </c>
       <c r="D16" s="20"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4">
       <c r="A17" s="19" t="s">
         <v>3</v>
       </c>
@@ -15524,7 +15688,7 @@
       </c>
       <c r="D17" s="20"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4">
       <c r="A18" s="19" t="s">
         <v>281</v>
       </c>
@@ -15535,7 +15699,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="32.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="32.4">
       <c r="A19" s="19" t="s">
         <v>281</v>
       </c>
@@ -15562,24 +15726,24 @@
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.2"/>
   <cols>
     <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" hidden="1">
       <c r="B2" s="16" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="16"/>
     </row>
-    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" hidden="1">
       <c r="B3" s="16" t="s">
         <v>151</v>
       </c>
@@ -15587,7 +15751,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" hidden="1">
       <c r="B4" s="16" t="s">
         <v>152</v>
       </c>
@@ -15595,7 +15759,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" hidden="1">
       <c r="B5" s="16" t="s">
         <v>153</v>
       </c>
@@ -15603,7 +15767,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" hidden="1">
       <c r="B6" s="16" t="s">
         <v>211</v>
       </c>
@@ -15611,7 +15775,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" hidden="1">
       <c r="B7" s="16" t="s">
         <v>212</v>
       </c>
@@ -15619,7 +15783,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" hidden="1">
       <c r="B8" s="16" t="s">
         <v>154</v>
       </c>
@@ -15627,13 +15791,13 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" hidden="1">
       <c r="B9" s="16" t="s">
         <v>67</v>
       </c>
       <c r="C9" s="16"/>
     </row>
-    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" hidden="1">
       <c r="B10" s="16" t="s">
         <v>155</v>
       </c>
@@ -15641,7 +15805,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" hidden="1">
       <c r="B11" s="16" t="s">
         <v>156</v>
       </c>
@@ -15649,7 +15813,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>224</v>
       </c>
@@ -15660,7 +15824,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>224</v>
       </c>
@@ -15671,7 +15835,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>224</v>
       </c>
@@ -15682,7 +15846,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" hidden="1">
       <c r="B15" s="16" t="s">
         <v>160</v>
       </c>
@@ -15690,7 +15854,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>137</v>
       </c>
@@ -15701,7 +15865,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>224</v>
       </c>
@@ -15712,7 +15876,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>224</v>
       </c>
@@ -15723,7 +15887,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" hidden="1">
       <c r="B19" s="16" t="s">
         <v>164</v>
       </c>
@@ -15731,7 +15895,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>224</v>
       </c>
@@ -15742,13 +15906,13 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" hidden="1">
       <c r="B21" s="16" t="s">
         <v>35</v>
       </c>
       <c r="C21" s="16"/>
     </row>
-    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" hidden="1">
       <c r="B22" s="16" t="s">
         <v>0</v>
       </c>
@@ -15756,7 +15920,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" hidden="1">
       <c r="B23" s="16" t="s">
         <v>166</v>
       </c>
@@ -15764,7 +15928,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" hidden="1">
       <c r="B24" s="16" t="s">
         <v>167</v>
       </c>
@@ -15772,7 +15936,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>224</v>
       </c>
@@ -15783,7 +15947,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>224</v>
       </c>
@@ -15794,7 +15958,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>224</v>
       </c>
@@ -15805,13 +15969,13 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" hidden="1">
       <c r="B28" s="16" t="s">
         <v>36</v>
       </c>
       <c r="C28" s="16"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>137</v>
       </c>
@@ -15822,7 +15986,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>224</v>
       </c>
@@ -15833,7 +15997,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>224</v>
       </c>
@@ -15844,13 +16008,13 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" hidden="1">
       <c r="B32" s="16" t="s">
         <v>39</v>
       </c>
       <c r="C32" s="16"/>
     </row>
-    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" hidden="1">
       <c r="B33" s="16" t="s">
         <v>174</v>
       </c>
@@ -15858,7 +16022,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>224</v>
       </c>
@@ -15869,7 +16033,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" hidden="1">
       <c r="B35" s="16" t="s">
         <v>175</v>
       </c>
@@ -15877,7 +16041,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" hidden="1">
       <c r="B36" s="16" t="s">
         <v>214</v>
       </c>
@@ -15885,13 +16049,13 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" hidden="1">
       <c r="B37" s="16" t="s">
         <v>142</v>
       </c>
       <c r="C37" s="16"/>
     </row>
-    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" hidden="1">
       <c r="B38" s="16" t="s">
         <v>177</v>
       </c>
@@ -15899,7 +16063,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" hidden="1">
       <c r="B39" s="16" t="s">
         <v>178</v>
       </c>
@@ -15907,7 +16071,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" hidden="1">
       <c r="B40" s="16" t="s">
         <v>179</v>
       </c>
@@ -15915,7 +16079,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" hidden="1">
       <c r="B41" s="16" t="s">
         <v>180</v>
       </c>
@@ -15923,13 +16087,13 @@
         <v>216</v>
       </c>
     </row>
-    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" hidden="1">
       <c r="B42" s="16" t="s">
         <v>38</v>
       </c>
       <c r="C42" s="16"/>
     </row>
-    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" hidden="1">
       <c r="B43" s="16" t="s">
         <v>135</v>
       </c>
@@ -15937,7 +16101,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" hidden="1">
       <c r="B44" s="16" t="s">
         <v>181</v>
       </c>
@@ -15945,7 +16109,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
         <v>224</v>
       </c>
@@ -15956,7 +16120,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" hidden="1">
       <c r="B46" s="16" t="s">
         <v>183</v>
       </c>
@@ -15964,7 +16128,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
         <v>137</v>
       </c>
@@ -15975,7 +16139,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" hidden="1">
       <c r="B48" s="16" t="s">
         <v>185</v>
       </c>
@@ -15983,7 +16147,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>137</v>
       </c>
@@ -15994,7 +16158,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>137</v>
       </c>
@@ -16005,7 +16169,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" hidden="1">
       <c r="B51" s="16" t="s">
         <v>187</v>
       </c>
@@ -16013,7 +16177,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" hidden="1">
       <c r="B52" s="16" t="s">
         <v>188</v>
       </c>
@@ -16021,7 +16185,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" hidden="1">
       <c r="B53" s="16" t="s">
         <v>189</v>
       </c>
@@ -16029,13 +16193,13 @@
         <v>104</v>
       </c>
     </row>
-    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" hidden="1">
       <c r="B54" s="16" t="s">
         <v>37</v>
       </c>
       <c r="C54" s="16"/>
     </row>
-    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" hidden="1">
       <c r="B55" s="16" t="s">
         <v>190</v>
       </c>
@@ -16043,7 +16207,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" hidden="1">
       <c r="B56" s="16" t="s">
         <v>191</v>
       </c>
@@ -16051,7 +16215,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" hidden="1">
       <c r="B57" s="16" t="s">
         <v>192</v>
       </c>
@@ -16059,7 +16223,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3">
       <c r="A58" t="s">
         <v>137</v>
       </c>
@@ -16070,13 +16234,13 @@
         <v>108</v>
       </c>
     </row>
-    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" hidden="1">
       <c r="B59" s="16" t="s">
         <v>34</v>
       </c>
       <c r="C59" s="16"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3">
       <c r="A60" t="s">
         <v>137</v>
       </c>
@@ -16087,7 +16251,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3">
       <c r="A61" t="s">
         <v>137</v>
       </c>
@@ -16098,7 +16262,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3">
       <c r="A62" t="s">
         <v>137</v>
       </c>
@@ -16109,7 +16273,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3">
       <c r="A63" t="s">
         <v>137</v>
       </c>
@@ -16120,7 +16284,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3">
       <c r="A64" t="s">
         <v>137</v>
       </c>
@@ -16131,7 +16295,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3">
       <c r="A65" t="s">
         <v>137</v>
       </c>
@@ -16142,13 +16306,13 @@
         <v>114</v>
       </c>
     </row>
-    <row r="66" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" hidden="1">
       <c r="B66" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C66" s="16"/>
     </row>
-    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" hidden="1">
       <c r="B67" s="16" t="s">
         <v>200</v>
       </c>
@@ -16156,7 +16320,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" hidden="1">
       <c r="B68" s="16" t="s">
         <v>201</v>
       </c>
@@ -16164,7 +16328,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" hidden="1">
       <c r="B69" s="16" t="s">
         <v>202</v>
       </c>
@@ -16172,7 +16336,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" hidden="1">
       <c r="B70" s="16" t="s">
         <v>203</v>
       </c>
@@ -16180,7 +16344,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="71" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" hidden="1">
       <c r="B71" s="16" t="s">
         <v>204</v>
       </c>
@@ -16188,7 +16352,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" hidden="1">
       <c r="B72" s="16" t="s">
         <v>205</v>
       </c>
@@ -16196,7 +16360,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" hidden="1">
       <c r="B73" s="16" t="s">
         <v>206</v>
       </c>
@@ -16204,7 +16368,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" hidden="1">
       <c r="B74" s="16" t="s">
         <v>207</v>
       </c>
@@ -16212,7 +16376,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" hidden="1">
       <c r="B75" s="16" t="s">
         <v>208</v>
       </c>
@@ -16220,7 +16384,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" hidden="1">
       <c r="B76" s="16" t="s">
         <v>209</v>
       </c>
@@ -16228,7 +16392,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="77" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" hidden="1">
       <c r="B77" s="16" t="s">
         <v>210</v>
       </c>
@@ -16236,13 +16400,13 @@
         <v>125</v>
       </c>
     </row>
-    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" hidden="1">
       <c r="B78" s="16" t="s">
         <v>3</v>
       </c>
       <c r="C78" s="16"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3">
       <c r="A79" t="s">
         <v>137</v>
       </c>

</xml_diff>